<commit_message>
Editing the README to try out git add/commit
</commit_message>
<xml_diff>
--- a/covidMNE2703.xlsx
+++ b/covidMNE2703.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dovla/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dovla/Desktop/covid19-mne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AE9E8E-2445-BD49-A8ED-B0B494ACCEC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED75CE18-C462-CB4B-AA2F-B8F4B46E196A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
   <si>
     <t>Country</t>
   </si>
@@ -902,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1251,7 +1251,7 @@
         <v>4</v>
       </c>
       <c r="G12">
-        <f t="shared" ref="G12:G20" si="0">E12-E11</f>
+        <f t="shared" ref="G12:G21" si="0">E12-E11</f>
         <v>8</v>
       </c>
       <c r="H12">
@@ -1278,7 +1278,7 @@
         <v>13</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:F20" si="1">(E13-E12)/E12</f>
+        <f t="shared" ref="F13:F21" si="1">(E13-E12)/E12</f>
         <v>0.3</v>
       </c>
       <c r="G13">
@@ -1508,6 +1508,37 @@
         <v>1</v>
       </c>
       <c r="I20">
+        <v>6278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43918</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>385</v>
+      </c>
+      <c r="E21">
+        <v>84</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
         <v>6278</v>
       </c>
     </row>

</xml_diff>